<commit_message>
Big Update - HIV Surveillance manager now tracks source, url, details - Updated nested likelihoods to draw parameters from surveillance data (for diff between counties or states vs MSAs) - Implemented MCMC for expanded continuum - Tweaks to plots and tables
</commit_message>
<xml_diff>
--- a/raw_data/local_continuum/processed/Cincinnati.xlsx
+++ b/raw_data/local_continuum/processed/Cincinnati.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd Fojo\CloudStation\Projects\Ending HIV\Ending_HIV\raw_data\local_continuum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd Fojo\CloudStation\Projects\Ending HIV\Ending_HIV\raw_data\local_continuum\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="87">
   <si>
     <t>Total</t>
   </si>
@@ -321,13 +321,19 @@
   </si>
   <si>
     <t>Ohio data</t>
+  </si>
+  <si>
+    <t>Has 2 counties not in MSA (Clinton, Highland) that have &lt;3% as many cases as in the other 5</t>
+  </si>
+  <si>
+    <t>Region (has 5 out of 16 counties from the MSA): Brown, Butler, Clermont, Hamilton, Warren - with &gt; 85% of the prevalent cases in MSA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +360,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -503,7 +516,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -583,6 +596,7 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -882,10 +896,10 @@
   <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R18" sqref="R18"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2190,10 +2204,14 @@
       <c r="Y18" s="15"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B20" s="15"/>
+      <c r="B20" s="51" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B21" s="15"/>
+      <c r="B21" s="15" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B22" s="15"/>
@@ -2533,7 +2551,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Big Update - HIV Surveillance manager tracks source, urls, details of data - Nested likelihoods use surveillance data to estimate parameters (instead of plugged in guesses) - Updated surveillance data XL files - Tweaks to tables/plots - MCMC for expanded continuum
</commit_message>
<xml_diff>
--- a/raw_data/local_continuum/processed/Cincinnati.xlsx
+++ b/raw_data/local_continuum/processed/Cincinnati.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd Fojo\CloudStation\Projects\Ending HIV\Ending_HIV\raw_data\local_continuum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd Fojo\CloudStation\Projects\Ending HIV\Ending_HIV\raw_data\local_continuum\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="87">
   <si>
     <t>Total</t>
   </si>
@@ -321,13 +321,19 @@
   </si>
   <si>
     <t>Ohio data</t>
+  </si>
+  <si>
+    <t>Has 2 counties not in MSA (Clinton, Highland) that have &lt;3% as many cases as in the other 5</t>
+  </si>
+  <si>
+    <t>Region (has 5 out of 16 counties from the MSA): Brown, Butler, Clermont, Hamilton, Warren - with &gt; 85% of the prevalent cases in MSA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +360,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -503,7 +516,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -583,6 +596,7 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -882,10 +896,10 @@
   <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R18" sqref="R18"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2190,10 +2204,14 @@
       <c r="Y18" s="15"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B20" s="15"/>
+      <c r="B20" s="51" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B21" s="15"/>
+      <c r="B21" s="15" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B22" s="15"/>
@@ -2533,7 +2551,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>